<commit_message>
Find the highest and lowest temperatures
</commit_message>
<xml_diff>
--- a/lemonade_analysis.xlsx
+++ b/lemonade_analysis.xlsx
@@ -101,7 +101,37 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="9">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -137,17 +167,17 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:I33" totalsRowCount="1">
   <autoFilter ref="A1:I32"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Date" dataDxfId="5" totalsRowDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="8" totalsRowDxfId="5"/>
     <tableColumn id="2" name="Location"/>
     <tableColumn id="3" name="Lemon"/>
     <tableColumn id="4" name="Orange"/>
     <tableColumn id="5" name="Temperature"/>
     <tableColumn id="6" name="Leaflets"/>
     <tableColumn id="7" name="Price"/>
-    <tableColumn id="8" name="Sales" dataDxfId="4" totalsRowDxfId="1">
+    <tableColumn id="8" name="Sales" dataDxfId="7" totalsRowDxfId="4">
       <calculatedColumnFormula>SUM(Tableau1[[#This Row],[Lemon]],Tableau1[[#This Row],[Orange]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Revenue" totalsRowFunction="custom" dataDxfId="3" totalsRowDxfId="0">
+    <tableColumn id="9" name="Revenue" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="3">
       <calculatedColumnFormula>Tableau1[[#This Row],[Sales]]*Tableau1[[#This Row],[Price]]</calculatedColumnFormula>
       <totalsRowFormula>SUM(Tableau1[Revenue])</totalsRowFormula>
     </tableColumn>
@@ -455,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1469,6 +1499,10 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2:E32">
+    <cfRule type="top10" dxfId="0" priority="2" percent="1" rank="10"/>
+    <cfRule type="top10" dxfId="1" priority="1" percent="1" bottom="1" rank="10"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Compare sales of Lemon and Orange flavors
</commit_message>
<xml_diff>
--- a/lemonade_analysis.xlsx
+++ b/lemonade_analysis.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
-    <sheet name="Dataset" sheetId="1" r:id="rId1"/>
-    <sheet name="Descriptive stats" sheetId="3" r:id="rId2"/>
-    <sheet name="Correlation" sheetId="4" r:id="rId3"/>
+    <sheet name="Lemon VS Orange" sheetId="5" r:id="rId1"/>
+    <sheet name="Dataset" sheetId="1" r:id="rId2"/>
+    <sheet name="Descriptive stats" sheetId="3" r:id="rId3"/>
+    <sheet name="Correlation" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">Dataset!$I$1</definedName>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -103,6 +104,39 @@
   </si>
   <si>
     <t>Nombre d'échantillons</t>
+  </si>
+  <si>
+    <t>Test d'égalité des espérances: deux observations de variances égales</t>
+  </si>
+  <si>
+    <t>Variance</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>Variance pondérée</t>
+  </si>
+  <si>
+    <t>Différence hypothétique des moyennes</t>
+  </si>
+  <si>
+    <t>Degré de liberté</t>
+  </si>
+  <si>
+    <t>Statistique t</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) unilatéral</t>
+  </si>
+  <si>
+    <t>Valeur critique de t (unilatéral)</t>
+  </si>
+  <si>
+    <t>P(T&lt;=t) bilatéral</t>
+  </si>
+  <si>
+    <t>Valeur critique de t (bilatéral)</t>
   </si>
 </sst>
 </file>
@@ -3538,10 +3572,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="58.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3">
+        <v>116.58064516129032</v>
+      </c>
+      <c r="C4" s="3">
+        <v>80.354838709677423</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3">
+        <v>683.11827956989293</v>
+      </c>
+      <c r="C5" s="3">
+        <v>489.7698924731182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3">
+        <v>586.44408602150554</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3">
+        <v>60</v>
+      </c>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="3">
+        <v>5.8893939518238767</v>
+      </c>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3">
+        <v>9.3931126296514368E-8</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.6706488649046354</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1.8786225259302874E-7</v>
+      </c>
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="4">
+        <v>2.0002978220142609</v>
+      </c>
+      <c r="C14" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:H32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4567,7 +4741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -4958,11 +5132,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>

</xml_diff>